<commit_message>
Query Sheet has been changed.
</commit_message>
<xml_diff>
--- a/release/queries.xlsx
+++ b/release/queries.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp1.0\www\prescription\release\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="6"/>
   </bookViews>
@@ -15,7 +20,7 @@
     <sheet name="alter chamber_id" sheetId="6" r:id="rId6"/>
     <sheet name="insert records from other table" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -397,8 +402,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,6 +448,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -489,7 +502,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,9 +534,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -555,6 +586,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -730,20 +779,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -808,7 +857,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -854,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -900,7 +949,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -946,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>23</v>
       </c>
@@ -992,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -1084,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -1130,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -1176,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -1222,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -1268,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1314,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1360,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1406,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>42</v>
       </c>
@@ -1452,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>45</v>
       </c>
@@ -1498,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>47</v>
       </c>
@@ -1544,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>50</v>
       </c>
@@ -1590,7 +1639,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>51</v>
       </c>
@@ -1636,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>54</v>
       </c>
@@ -1682,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>55</v>
       </c>
@@ -1728,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1757,19 +1806,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1830,7 +1879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -1868,7 +1917,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -1906,7 +1955,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -1944,7 +1993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -1982,7 +2031,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
@@ -2020,7 +2069,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -2058,7 +2107,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>31</v>
       </c>
@@ -2096,7 +2145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>34</v>
       </c>
@@ -2134,7 +2183,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>35</v>
       </c>
@@ -2172,7 +2221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:13">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -2210,7 +2259,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>39</v>
       </c>
@@ -2248,7 +2297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:13">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>42</v>
       </c>
@@ -2286,7 +2335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>45</v>
       </c>
@@ -2324,7 +2373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:13">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>47</v>
       </c>
@@ -2362,7 +2411,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>51</v>
       </c>
@@ -2400,7 +2449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>54</v>
       </c>
@@ -2438,7 +2487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>55</v>
       </c>
@@ -2476,7 +2525,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -2505,16 +2554,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K43"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>78</v>
       </c>
@@ -2537,7 +2586,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>78</v>
       </c>
@@ -2560,7 +2609,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>78</v>
       </c>
@@ -2583,7 +2632,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>78</v>
       </c>
@@ -2606,7 +2655,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
         <v>80</v>
       </c>
@@ -2620,7 +2669,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>83</v>
       </c>
@@ -2646,7 +2695,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>80</v>
       </c>
@@ -2660,7 +2709,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>83</v>
       </c>
@@ -2686,7 +2735,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>83</v>
       </c>
@@ -2712,7 +2761,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>83</v>
       </c>
@@ -2738,7 +2787,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>83</v>
       </c>
@@ -2764,7 +2813,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>83</v>
       </c>
@@ -2790,7 +2839,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>83</v>
       </c>
@@ -2816,7 +2865,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>83</v>
       </c>
@@ -2842,7 +2891,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>83</v>
       </c>
@@ -2868,7 +2917,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>83</v>
       </c>
@@ -2894,7 +2943,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>83</v>
       </c>
@@ -2920,7 +2969,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>83</v>
       </c>
@@ -2946,7 +2995,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>83</v>
       </c>
@@ -2960,7 +3009,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>83</v>
       </c>
@@ -2974,7 +3023,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>83</v>
       </c>
@@ -2988,7 +3037,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>83</v>
       </c>
@@ -3002,7 +3051,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>83</v>
       </c>
@@ -3016,7 +3065,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>85</v>
       </c>
@@ -3042,7 +3091,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>85</v>
       </c>
@@ -3068,7 +3117,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>85</v>
       </c>
@@ -3094,7 +3143,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:11">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>85</v>
       </c>
@@ -3120,7 +3169,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:11">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>85</v>
       </c>
@@ -3146,7 +3195,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>85</v>
       </c>
@@ -3172,7 +3221,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>85</v>
       </c>
@@ -3198,7 +3247,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>85</v>
       </c>
@@ -3224,7 +3273,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>85</v>
       </c>
@@ -3250,7 +3299,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>85</v>
       </c>
@@ -3276,7 +3325,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>85</v>
       </c>
@@ -3302,7 +3351,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>85</v>
       </c>
@@ -3328,7 +3377,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>85</v>
       </c>
@@ -3354,7 +3403,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>85</v>
       </c>
@@ -3380,7 +3429,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>85</v>
       </c>
@@ -3406,7 +3455,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>85</v>
       </c>
@@ -3432,7 +3481,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="2:9">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>85</v>
       </c>
@@ -3464,19 +3513,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>112</v>
       </c>
@@ -3484,7 +3533,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>112</v>
       </c>
@@ -3492,7 +3541,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>112</v>
       </c>
@@ -3506,7 +3555,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>112</v>
       </c>
@@ -3520,7 +3569,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>112</v>
       </c>
@@ -3534,7 +3583,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>112</v>
       </c>
@@ -3548,7 +3597,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>112</v>
       </c>
@@ -3562,7 +3611,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>112</v>
       </c>
@@ -3576,7 +3625,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>112</v>
       </c>
@@ -3590,7 +3639,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>112</v>
       </c>
@@ -3604,7 +3653,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>112</v>
       </c>
@@ -3618,7 +3667,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>112</v>
       </c>
@@ -3632,7 +3681,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>112</v>
       </c>
@@ -3646,7 +3695,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>112</v>
       </c>
@@ -3660,7 +3709,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>112</v>
       </c>
@@ -3674,7 +3723,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>112</v>
       </c>
@@ -3688,7 +3737,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>112</v>
       </c>
@@ -3702,7 +3751,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>112</v>
       </c>
@@ -3716,7 +3765,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>112</v>
       </c>
@@ -3730,7 +3779,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>112</v>
       </c>
@@ -3744,7 +3793,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>112</v>
       </c>
@@ -3758,7 +3807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>112</v>
       </c>
@@ -3772,7 +3821,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>112</v>
       </c>
@@ -3786,7 +3835,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>112</v>
       </c>
@@ -3800,7 +3849,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>112</v>
       </c>
@@ -3814,7 +3863,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>112</v>
       </c>
@@ -3834,19 +3883,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -3860,7 +3909,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -3874,7 +3923,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -3888,7 +3937,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -3902,7 +3951,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -3916,7 +3965,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -3930,7 +3979,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3944,7 +3993,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -3958,7 +4007,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -3972,7 +4021,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -3986,7 +4035,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -4000,7 +4049,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -4014,7 +4063,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -4028,7 +4077,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -4042,7 +4091,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -4056,7 +4105,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -4076,19 +4125,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -4102,7 +4151,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -4116,7 +4165,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -4130,7 +4179,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -4144,7 +4193,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4158,7 +4207,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -4172,7 +4221,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -4186,7 +4235,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -4200,7 +4249,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -4214,7 +4263,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -4228,7 +4277,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -4242,7 +4291,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -4256,7 +4305,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -4270,7 +4319,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -4284,7 +4333,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -4298,7 +4347,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -4318,19 +4367,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C23"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -4341,7 +4390,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -4352,7 +4401,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -4363,7 +4412,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -4374,7 +4423,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -4385,7 +4434,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -4396,7 +4445,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -4407,7 +4456,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -4418,7 +4467,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -4429,7 +4478,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -4440,7 +4489,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -4451,7 +4500,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -4462,7 +4511,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -4473,7 +4522,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -4484,7 +4533,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -4495,7 +4544,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -4506,7 +4555,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -4517,7 +4566,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -4528,7 +4577,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>80</v>
       </c>
@@ -4539,7 +4588,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -4550,7 +4599,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -4561,7 +4610,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -4572,7 +4621,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>80</v>
       </c>

</xml_diff>